<commit_message>
hoac on ni uptake
</commit_message>
<xml_diff>
--- a/HOAc work/Ni(110)/Acetic Acid Area_output 5_16_18.xlsx
+++ b/HOAc work/Ni(110)/Acetic Acid Area_output 5_16_18.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manolis\Desktop\PycharmProjects\IRAS\IRAS\HOAc work\Ni(110)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9DC887-A945-4862-8014-B02A3E4CBB65}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331CC21F-B7DA-4331-B090-4C27D3AACFB1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -831,7 +831,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$2</c15:sqref>
@@ -872,7 +872,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$3:$I$18</c15:sqref>
@@ -935,7 +935,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$3:$L$18</c15:sqref>
@@ -997,7 +997,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-73A4-4DD5-B69E-ED66D9286026}"/>
                   </c:ext>
@@ -1396,6 +1396,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="489857328"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2078,7 +2079,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$U$2</c15:sqref>
@@ -2119,7 +2120,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$S$3:$S$18</c15:sqref>
@@ -2182,7 +2183,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$U$3:$U$18</c15:sqref>
@@ -2244,7 +2245,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-2603-488E-831D-631D312D14D6}"/>
                   </c:ext>
@@ -2643,6 +2644,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="489856464"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3324,7 +3326,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$22</c15:sqref>
@@ -3365,7 +3367,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$23:$I$38</c15:sqref>
@@ -3428,7 +3430,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$23:$L$38</c15:sqref>
@@ -3490,7 +3492,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-9B82-4180-B01F-D32B4BDA539B}"/>
                   </c:ext>
@@ -3857,6 +3859,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="489872016"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -5650,16 +5653,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>552796</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>120535</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>253538</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>153786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>145472</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>187037</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>511232</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>29095</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5687,15 +5690,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1404850</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>1172094</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>153785</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>448887</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>12469</xdr:rowOff>
+      <xdr:colOff>216131</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>29094</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6046,8 +6049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -6181,7 +6184,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <f>O3-0.1*N3</f>
+        <f t="shared" ref="P3:P18" si="0">O3-0.1*N3</f>
         <v>0</v>
       </c>
       <c r="R3">
@@ -6206,7 +6209,7 @@
         <v>0</v>
       </c>
       <c r="Y3">
-        <f>X3-0.1*W3</f>
+        <f t="shared" ref="Y3:Y18" si="1">X3-0.1*W3</f>
         <v>0</v>
       </c>
     </row>
@@ -6230,7 +6233,7 @@
         <v>5077998.7396892207</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G17" si="0">F4-0.1*E4</f>
+        <f t="shared" ref="G4:G17" si="2">F4-0.1*E4</f>
         <v>4322069.0458857054</v>
       </c>
       <c r="I4">
@@ -6255,7 +6258,7 @@
         <v>8063029.9839975797</v>
       </c>
       <c r="P4">
-        <f>O4-0.1*N4</f>
+        <f t="shared" si="0"/>
         <v>6932903.8475196017</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -6281,7 +6284,7 @@
         <v>5077998.7396892207</v>
       </c>
       <c r="Y4">
-        <f>X4-0.1*W4</f>
+        <f t="shared" si="1"/>
         <v>4322069.0458857054</v>
       </c>
     </row>
@@ -6305,7 +6308,7 @@
         <v>13585008.49200085</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11956488.186511599</v>
       </c>
       <c r="I5">
@@ -6330,7 +6333,7 @@
         <v>5077998.7396892207</v>
       </c>
       <c r="P5">
-        <f>O5-0.1*N5</f>
+        <f t="shared" si="0"/>
         <v>4322069.0458857054</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -6356,7 +6359,7 @@
         <v>7971459.8616463887</v>
       </c>
       <c r="Y5">
-        <f>X5-0.1*W5</f>
+        <f t="shared" si="1"/>
         <v>6819427.8665669663</v>
       </c>
     </row>
@@ -6380,7 +6383,7 @@
         <v>13434788.10757477</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11813398.796008855</v>
       </c>
       <c r="I6">
@@ -6405,7 +6408,7 @@
         <v>7971459.8616463887</v>
       </c>
       <c r="P6">
-        <f>O6-0.1*N6</f>
+        <f t="shared" si="0"/>
         <v>6819427.8665669663</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -6431,7 +6434,7 @@
         <v>8063029.9839975797</v>
       </c>
       <c r="Y6">
-        <f>X6-0.1*W6</f>
+        <f t="shared" si="1"/>
         <v>6932903.8475196017</v>
       </c>
     </row>
@@ -6455,7 +6458,7 @@
         <v>7971459.8616463887</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6819427.8665669663</v>
       </c>
       <c r="I7">
@@ -6480,7 +6483,7 @@
         <v>10600218.147781439</v>
       </c>
       <c r="P7">
-        <f>O7-0.1*N7</f>
+        <f t="shared" si="0"/>
         <v>9177764.8321971819</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -6506,7 +6509,7 @@
         <v>10600218.147781439</v>
       </c>
       <c r="Y7">
-        <f>X7-0.1*W7</f>
+        <f t="shared" si="1"/>
         <v>9177764.8321971819</v>
       </c>
     </row>
@@ -6530,7 +6533,7 @@
         <v>8063029.9839975797</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6932903.8475196017</v>
       </c>
       <c r="I8">
@@ -6555,7 +6558,7 @@
         <v>10838513.314139459</v>
       </c>
       <c r="P8">
-        <f>O8-0.1*N8</f>
+        <f t="shared" si="0"/>
         <v>9356076.2782120463</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -6581,7 +6584,7 @@
         <v>10838513.314139459</v>
       </c>
       <c r="Y8">
-        <f>X8-0.1*W8</f>
+        <f t="shared" si="1"/>
         <v>9356076.2782120463</v>
       </c>
     </row>
@@ -6605,7 +6608,7 @@
         <v>10600218.147781439</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9177764.8321971819</v>
       </c>
       <c r="I9">
@@ -6630,7 +6633,7 @@
         <v>11977008.39862336</v>
       </c>
       <c r="P9">
-        <f>O9-0.1*N9</f>
+        <f t="shared" si="0"/>
         <v>10422779.796747554</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -6656,7 +6659,7 @@
         <v>12872728.71279531</v>
       </c>
       <c r="Y9">
-        <f>X9-0.1*W9</f>
+        <f t="shared" si="1"/>
         <v>11142338.399305219</v>
       </c>
     </row>
@@ -6680,7 +6683,7 @@
         <v>10838513.314139459</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9356076.2782120463</v>
       </c>
       <c r="I10">
@@ -6705,7 +6708,7 @@
         <v>12872728.71279531</v>
       </c>
       <c r="P10">
-        <f>O10-0.1*N10</f>
+        <f t="shared" si="0"/>
         <v>11142338.399305219</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -6731,7 +6734,7 @@
         <v>11977008.39862336</v>
       </c>
       <c r="Y10">
-        <f>X10-0.1*W10</f>
+        <f t="shared" si="1"/>
         <v>10422779.796747554</v>
       </c>
     </row>
@@ -6755,7 +6758,7 @@
         <v>12872728.71279531</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11142338.399305219</v>
       </c>
       <c r="I11">
@@ -6780,7 +6783,7 @@
         <v>12280105.25103936</v>
       </c>
       <c r="P11">
-        <f>O11-0.1*N11</f>
+        <f t="shared" si="0"/>
         <v>10820401.835562717</v>
       </c>
       <c r="R11" s="1" t="s">
@@ -6806,7 +6809,7 @@
         <v>13387017.792110629</v>
       </c>
       <c r="Y11">
-        <f>X11-0.1*W11</f>
+        <f t="shared" si="1"/>
         <v>11708275.308671076</v>
       </c>
     </row>
@@ -6830,7 +6833,7 @@
         <v>11977008.39862336</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10422779.796747554</v>
       </c>
       <c r="I12">
@@ -6855,7 +6858,7 @@
         <v>13387017.792110629</v>
       </c>
       <c r="P12">
-        <f>O12-0.1*N12</f>
+        <f t="shared" si="0"/>
         <v>11708275.308671076</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -6881,7 +6884,7 @@
         <v>12280105.25103936</v>
       </c>
       <c r="Y12">
-        <f>X12-0.1*W12</f>
+        <f t="shared" si="1"/>
         <v>10820401.835562717</v>
       </c>
     </row>
@@ -6905,7 +6908,7 @@
         <v>13387017.792110629</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11708275.308671076</v>
       </c>
       <c r="I13">
@@ -6930,7 +6933,7 @@
         <v>12206096.30309541</v>
       </c>
       <c r="P13">
-        <f>O13-0.1*N13</f>
+        <f t="shared" si="0"/>
         <v>10658897.834186198</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -6956,7 +6959,7 @@
         <v>13138063.60631272</v>
       </c>
       <c r="Y13">
-        <f>X13-0.1*W13</f>
+        <f t="shared" si="1"/>
         <v>11482444.267947793</v>
       </c>
     </row>
@@ -6980,7 +6983,7 @@
         <v>12280105.25103936</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10820401.835562717</v>
       </c>
       <c r="I14">
@@ -7005,7 +7008,7 @@
         <v>12903431.32376256</v>
       </c>
       <c r="P14">
-        <f>O14-0.1*N14</f>
+        <f t="shared" si="0"/>
         <v>11346352.185566513</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -7031,7 +7034,7 @@
         <v>12903431.32376256</v>
       </c>
       <c r="Y14">
-        <f>X14-0.1*W14</f>
+        <f t="shared" si="1"/>
         <v>11346352.185566513</v>
       </c>
     </row>
@@ -7055,7 +7058,7 @@
         <v>13138063.60631272</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11482444.267947793</v>
       </c>
       <c r="I15">
@@ -7080,7 +7083,7 @@
         <v>13585008.49200085</v>
       </c>
       <c r="P15">
-        <f>O15-0.1*N15</f>
+        <f t="shared" si="0"/>
         <v>11956488.186511599</v>
       </c>
       <c r="R15" s="1" t="s">
@@ -7106,7 +7109,7 @@
         <v>12206096.30309541</v>
       </c>
       <c r="Y15">
-        <f>X15-0.1*W15</f>
+        <f t="shared" si="1"/>
         <v>10658897.834186198</v>
       </c>
     </row>
@@ -7130,7 +7133,7 @@
         <v>12903431.32376256</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11346352.185566513</v>
       </c>
       <c r="I16">
@@ -7155,7 +7158,7 @@
         <v>13519583.027904641</v>
       </c>
       <c r="P16">
-        <f>O16-0.1*N16</f>
+        <f t="shared" si="0"/>
         <v>11882760.899278512</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -7181,7 +7184,7 @@
         <v>13585008.49200085</v>
       </c>
       <c r="Y16">
-        <f>X16-0.1*W16</f>
+        <f t="shared" si="1"/>
         <v>11956488.186511599</v>
       </c>
     </row>
@@ -7205,7 +7208,7 @@
         <v>12206096.30309541</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10658897.834186198</v>
       </c>
       <c r="I17">
@@ -7230,7 +7233,7 @@
         <v>13138063.60631272</v>
       </c>
       <c r="P17">
-        <f>O17-0.1*N17</f>
+        <f t="shared" si="0"/>
         <v>11482444.267947793</v>
       </c>
       <c r="R17" s="1" t="s">
@@ -7256,7 +7259,7 @@
         <v>13519583.027904641</v>
       </c>
       <c r="Y17">
-        <f>X17-0.1*W17</f>
+        <f t="shared" si="1"/>
         <v>11882760.899278512</v>
       </c>
     </row>
@@ -7305,7 +7308,7 @@
         <v>13434788.10757477</v>
       </c>
       <c r="P18">
-        <f>O18-0.1*N18</f>
+        <f t="shared" si="0"/>
         <v>11813398.796008855</v>
       </c>
       <c r="R18" s="1" t="s">
@@ -7331,7 +7334,7 @@
         <v>13434788.10757477</v>
       </c>
       <c r="Y18">
-        <f>X18-0.1*W18</f>
+        <f t="shared" si="1"/>
         <v>11813398.796008855</v>
       </c>
     </row>
@@ -7386,7 +7389,7 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <f>O23-0.1*N23</f>
+        <f t="shared" ref="P23:P38" si="3">O23-0.1*N23</f>
         <v>0</v>
       </c>
     </row>
@@ -7413,7 +7416,7 @@
         <v>5077998.7396892207</v>
       </c>
       <c r="P24">
-        <f>O24-0.1*N24</f>
+        <f t="shared" si="3"/>
         <v>4322069.0458857054</v>
       </c>
     </row>
@@ -7440,7 +7443,7 @@
         <v>8063029.9839975797</v>
       </c>
       <c r="P25">
-        <f>O25-0.1*N25</f>
+        <f t="shared" si="3"/>
         <v>6932903.8475196017</v>
       </c>
     </row>
@@ -7467,7 +7470,7 @@
         <v>7971459.8616463887</v>
       </c>
       <c r="P26">
-        <f>O26-0.1*N26</f>
+        <f t="shared" si="3"/>
         <v>6819427.8665669663</v>
       </c>
     </row>
@@ -7494,7 +7497,7 @@
         <v>10600218.147781439</v>
       </c>
       <c r="P27">
-        <f>O27-0.1*N27</f>
+        <f t="shared" si="3"/>
         <v>9177764.8321971819</v>
       </c>
     </row>
@@ -7521,7 +7524,7 @@
         <v>12280105.25103936</v>
       </c>
       <c r="P28">
-        <f>O28-0.1*N28</f>
+        <f t="shared" si="3"/>
         <v>10820401.835562717</v>
       </c>
     </row>
@@ -7548,7 +7551,7 @@
         <v>10838513.314139459</v>
       </c>
       <c r="P29">
-        <f>O29-0.1*N29</f>
+        <f t="shared" si="3"/>
         <v>9356076.2782120463</v>
       </c>
     </row>
@@ -7575,7 +7578,7 @@
         <v>12206096.30309541</v>
       </c>
       <c r="P30">
-        <f>O30-0.1*N30</f>
+        <f t="shared" si="3"/>
         <v>10658897.834186198</v>
       </c>
     </row>
@@ -7602,7 +7605,7 @@
         <v>11977008.39862336</v>
       </c>
       <c r="P31">
-        <f>O31-0.1*N31</f>
+        <f t="shared" si="3"/>
         <v>10422779.796747554</v>
       </c>
     </row>
@@ -7629,7 +7632,7 @@
         <v>12903431.32376256</v>
       </c>
       <c r="P32">
-        <f>O32-0.1*N32</f>
+        <f t="shared" si="3"/>
         <v>11346352.185566513</v>
       </c>
     </row>
@@ -7656,7 +7659,7 @@
         <v>13434788.10757477</v>
       </c>
       <c r="P33">
-        <f>O33-0.1*N33</f>
+        <f t="shared" si="3"/>
         <v>11813398.796008855</v>
       </c>
     </row>
@@ -7683,7 +7686,7 @@
         <v>13585008.49200085</v>
       </c>
       <c r="P34">
-        <f>O34-0.1*N34</f>
+        <f t="shared" si="3"/>
         <v>11956488.186511599</v>
       </c>
     </row>
@@ -7710,7 +7713,7 @@
         <v>13519583.027904641</v>
       </c>
       <c r="P35">
-        <f>O35-0.1*N35</f>
+        <f t="shared" si="3"/>
         <v>11882760.899278512</v>
       </c>
     </row>
@@ -7737,7 +7740,7 @@
         <v>13138063.60631272</v>
       </c>
       <c r="P36">
-        <f>O36-0.1*N36</f>
+        <f t="shared" si="3"/>
         <v>11482444.267947793</v>
       </c>
     </row>
@@ -7764,7 +7767,7 @@
         <v>13387017.792110629</v>
       </c>
       <c r="P37">
-        <f>O37-0.1*N37</f>
+        <f t="shared" si="3"/>
         <v>11708275.308671076</v>
       </c>
     </row>
@@ -7791,7 +7794,7 @@
         <v>12872728.71279531</v>
       </c>
       <c r="P38">
-        <f>O38-0.1*N38</f>
+        <f t="shared" si="3"/>
         <v>11142338.399305219</v>
       </c>
     </row>

</xml_diff>